<commit_message>
Create revisions to cleanup and streamline project
</commit_message>
<xml_diff>
--- a/project/access_control_matrix/Access_Control_Matrix.xlsx
+++ b/project/access_control_matrix/Access_Control_Matrix.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Subject (IAM Roles) /Object (AWS Resources)</t>
   </si>
@@ -25,7 +25,7 @@
     <t>CloudWatch monitoring</t>
   </si>
   <si>
-    <t>EC2 Monitoring</t>
+    <t>EC2</t>
   </si>
   <si>
     <t>S3 Buckets</t>
@@ -58,13 +58,16 @@
     <t>Read (objects with tag Stage and value of ObfuscatedReportReady)</t>
   </si>
   <si>
+    <t>Read/Write (objects with tag Role and value of analyst)</t>
+  </si>
+  <si>
     <t>Read Access (List all buckets)</t>
   </si>
   <si>
     <t>enterprise-developer-role</t>
   </si>
   <si>
-    <t>Read/Write (objects with tag Role and value of username)</t>
+    <t>Read/Write (objects with tag Role and value of developer)</t>
   </si>
   <si>
     <t>Read Access (List all Resources)</t>
@@ -74,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -82,6 +85,11 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -113,23 +121,29 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -356,6 +370,7 @@
     <col customWidth="1" min="6" max="6" width="34.86"/>
     <col customWidth="1" min="7" max="7" width="32.71"/>
     <col customWidth="1" min="8" max="8" width="72.71"/>
+    <col customWidth="1" min="9" max="9" width="31.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -368,10 +383,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -380,7 +395,7 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -388,25 +403,25 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -414,51 +429,51 @@
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>